<commit_message>
Wiremill building, localization, New Technologies
</commit_message>
<xml_diff>
--- a/IndustryExpanded/FACTORIES.xlsx
+++ b/IndustryExpanded/FACTORIES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3TO_9I\Documents\Paradox Interactive\Victoria 3\mod\IndustryExpanded\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F233E9-428F-446E-A66D-7AB80CB5CD15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF46470F-0B1F-4183-AFFC-85767C7CA033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8AEE59E-FFCD-4A72-B877-FD5D3ADEE5A1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="47">
   <si>
     <t>Building</t>
   </si>
@@ -162,6 +162,21 @@
   </si>
   <si>
     <t>Tier 4: Crystal, Plastic, Blowers</t>
+  </si>
+  <si>
+    <t>Wiremill</t>
+  </si>
+  <si>
+    <t>Tier 4: Electroplated, Rubber, Asslines</t>
+  </si>
+  <si>
+    <t>Tier 1: Solid Wire, Copper Cable, Manual</t>
+  </si>
+  <si>
+    <t>Tier 2: Stranded Twisting, Insulated, Pneumatic</t>
+  </si>
+  <si>
+    <t>Tier 3: Stranded Twisting, Rubber, Electric</t>
   </si>
 </sst>
 </file>
@@ -398,12 +413,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -412,6 +421,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -755,10 +770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{619B0D70-D2AF-46B3-9D3D-17ECB8467BBA}">
-  <dimension ref="A1:N65"/>
+  <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,7 +827,7 @@
       <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="24" t="s">
         <v>8</v>
       </c>
       <c r="G2" s="14">
@@ -834,7 +849,7 @@
       <c r="M2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="22" t="s">
+      <c r="N2" s="24" t="s">
         <v>13</v>
       </c>
     </row>
@@ -850,7 +865,7 @@
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="22"/>
+      <c r="F3" s="24"/>
       <c r="G3" s="16">
         <v>1200</v>
       </c>
@@ -867,7 +882,7 @@
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="9"/>
-      <c r="N3" s="22"/>
+      <c r="N3" s="24"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
@@ -887,7 +902,7 @@
       <c r="E4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="22"/>
+      <c r="F4" s="24"/>
       <c r="G4" s="15">
         <f>G3-G2</f>
         <v>600</v>
@@ -912,7 +927,7 @@
       <c r="M4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="22"/>
+      <c r="N4" s="24"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -931,7 +946,7 @@
       <c r="E5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="24" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="14">
@@ -954,7 +969,7 @@
       <c r="M5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="N5" s="22" t="s">
+      <c r="N5" s="24" t="s">
         <v>14</v>
       </c>
     </row>
@@ -971,7 +986,7 @@
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="22"/>
+      <c r="F6" s="24"/>
       <c r="G6" s="16">
         <v>2400</v>
       </c>
@@ -987,7 +1002,7 @@
       </c>
       <c r="L6" s="3"/>
       <c r="M6" s="9"/>
-      <c r="N6" s="22"/>
+      <c r="N6" s="24"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -1007,7 +1022,7 @@
       <c r="E7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="22"/>
+      <c r="F7" s="24"/>
       <c r="G7" s="15">
         <f>G6-G5</f>
         <v>800</v>
@@ -1032,7 +1047,7 @@
       <c r="M7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="N7" s="22"/>
+      <c r="N7" s="24"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -1051,7 +1066,7 @@
       <c r="E8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G8" s="14">
@@ -1074,7 +1089,7 @@
       <c r="M8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="N8" s="22" t="s">
+      <c r="N8" s="24" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1091,7 +1106,7 @@
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="9"/>
-      <c r="F9" s="22"/>
+      <c r="F9" s="24"/>
       <c r="G9" s="16">
         <v>3200</v>
       </c>
@@ -1108,7 +1123,7 @@
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="9"/>
-      <c r="N9" s="22"/>
+      <c r="N9" s="24"/>
     </row>
     <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
@@ -1128,7 +1143,7 @@
       <c r="E10" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="22"/>
+      <c r="F10" s="24"/>
       <c r="G10" s="15">
         <f>G9-G8</f>
         <v>1100</v>
@@ -1153,7 +1168,7 @@
       <c r="M10" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="N10" s="22"/>
+      <c r="N10" s="24"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
@@ -1172,7 +1187,7 @@
       <c r="E11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="24" t="s">
         <v>11</v>
       </c>
       <c r="G11" s="14">
@@ -1195,7 +1210,7 @@
       <c r="M11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="N11" s="22" t="s">
+      <c r="N11" s="24" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1212,7 +1227,7 @@
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="9"/>
-      <c r="F12" s="22"/>
+      <c r="F12" s="24"/>
       <c r="G12" s="16">
         <v>4200</v>
       </c>
@@ -1229,7 +1244,7 @@
       </c>
       <c r="L12" s="3"/>
       <c r="M12" s="9"/>
-      <c r="N12" s="22"/>
+      <c r="N12" s="24"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
@@ -1249,7 +1264,7 @@
       <c r="E13" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="22"/>
+      <c r="F13" s="24"/>
       <c r="G13" s="15">
         <f>G12-G11</f>
         <v>1800</v>
@@ -1274,7 +1289,7 @@
       <c r="M13" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="N13" s="22"/>
+      <c r="N13" s="24"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
@@ -1310,7 +1325,7 @@
       <c r="E15" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="24" t="s">
         <v>26</v>
       </c>
       <c r="G15" s="14">
@@ -1346,7 +1361,7 @@
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="9"/>
-      <c r="F16" s="22"/>
+      <c r="F16" s="24"/>
       <c r="G16" s="16">
         <v>1200</v>
       </c>
@@ -1381,7 +1396,7 @@
       <c r="E17" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="22"/>
+      <c r="F17" s="24"/>
       <c r="G17" s="15">
         <f>G16-G15</f>
         <v>600</v>
@@ -1423,7 +1438,7 @@
       <c r="E18" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="24" t="s">
         <v>25</v>
       </c>
       <c r="G18" s="14">
@@ -1460,7 +1475,7 @@
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="9"/>
-      <c r="F19" s="22"/>
+      <c r="F19" s="24"/>
       <c r="G19" s="16">
         <v>2400</v>
       </c>
@@ -1496,7 +1511,7 @@
       <c r="E20" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F20" s="22"/>
+      <c r="F20" s="24"/>
       <c r="G20" s="15">
         <f>G19-G18</f>
         <v>800</v>
@@ -1630,7 +1645,7 @@
       <c r="E24" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="22" t="s">
+      <c r="F24" s="24" t="s">
         <v>27</v>
       </c>
       <c r="G24" s="14">
@@ -1659,7 +1674,7 @@
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="9"/>
-      <c r="F25" s="22"/>
+      <c r="F25" s="24"/>
       <c r="G25" s="16">
         <v>4200</v>
       </c>
@@ -1689,7 +1704,7 @@
       <c r="E26" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="22"/>
+      <c r="F26" s="24"/>
       <c r="G26" s="15">
         <f>G25-G24</f>
         <v>1800</v>
@@ -1758,7 +1773,7 @@
       <c r="E31" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="22" t="s">
+      <c r="F31" s="24" t="s">
         <v>29</v>
       </c>
       <c r="G31" s="14">
@@ -1775,7 +1790,7 @@
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="9"/>
-      <c r="F32" s="22"/>
+      <c r="F32" s="24"/>
       <c r="G32" s="16">
         <v>2400</v>
       </c>
@@ -1797,7 +1812,7 @@
       <c r="E33" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F33" s="22"/>
+      <c r="F33" s="24"/>
       <c r="G33" s="15">
         <f>G32-G31</f>
         <v>800</v>
@@ -1821,7 +1836,7 @@
       <c r="E34" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F34" s="21" t="s">
+      <c r="F34" s="25" t="s">
         <v>31</v>
       </c>
       <c r="G34" s="14">
@@ -1839,7 +1854,7 @@
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="9"/>
-      <c r="F35" s="21"/>
+      <c r="F35" s="25"/>
       <c r="G35" s="16">
         <v>3200</v>
       </c>
@@ -1861,7 +1876,7 @@
       <c r="E36" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F36" s="21"/>
+      <c r="F36" s="25"/>
       <c r="G36" s="15">
         <f>G35-G34</f>
         <v>1100</v>
@@ -1885,7 +1900,7 @@
       <c r="E37" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F37" s="21" t="s">
+      <c r="F37" s="25" t="s">
         <v>30</v>
       </c>
       <c r="G37" s="14">
@@ -1902,7 +1917,7 @@
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="9"/>
-      <c r="F38" s="21"/>
+      <c r="F38" s="25"/>
       <c r="G38" s="16">
         <v>4200</v>
       </c>
@@ -1924,7 +1939,7 @@
       <c r="E39" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F39" s="21"/>
+      <c r="F39" s="25"/>
       <c r="G39" s="15">
         <f>G38-G37</f>
         <v>1800</v>
@@ -1951,7 +1966,7 @@
       <c r="A41" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>32</v>
       </c>
       <c r="C41" s="6">
@@ -1963,7 +1978,7 @@
       <c r="E41" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F41" s="22" t="s">
+      <c r="F41" s="24" t="s">
         <v>33</v>
       </c>
       <c r="G41" s="14">
@@ -1975,13 +1990,13 @@
       <c r="A42" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B42" s="24"/>
+      <c r="B42" s="22"/>
       <c r="C42" s="3">
         <v>1350</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="9"/>
-      <c r="F42" s="22"/>
+      <c r="F42" s="24"/>
       <c r="G42" s="16">
         <v>1200</v>
       </c>
@@ -1991,7 +2006,7 @@
       <c r="A43" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="25"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="12">
         <f>C42-C41</f>
         <v>550</v>
@@ -2003,7 +2018,7 @@
       <c r="E43" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F43" s="22"/>
+      <c r="F43" s="24"/>
       <c r="G43" s="15">
         <f>G42-G41</f>
         <v>600</v>
@@ -2016,7 +2031,7 @@
       <c r="A44" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B44" s="23" t="s">
+      <c r="B44" s="21" t="s">
         <v>32</v>
       </c>
       <c r="C44" s="6">
@@ -2029,7 +2044,7 @@
       <c r="E44" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F44" s="22" t="s">
+      <c r="F44" s="24" t="s">
         <v>34</v>
       </c>
       <c r="G44" s="14">
@@ -2041,13 +2056,13 @@
       <c r="A45" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B45" s="24"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="3">
         <v>2100</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="9"/>
-      <c r="F45" s="22"/>
+      <c r="F45" s="24"/>
       <c r="G45" s="16">
         <v>2400</v>
       </c>
@@ -2057,7 +2072,7 @@
       <c r="A46" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="25"/>
+      <c r="B46" s="23"/>
       <c r="C46" s="12">
         <f>C45-C44</f>
         <v>820</v>
@@ -2069,7 +2084,7 @@
       <c r="E46" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F46" s="22"/>
+      <c r="F46" s="24"/>
       <c r="G46" s="15">
         <f>G45-G44</f>
         <v>800</v>
@@ -2082,7 +2097,7 @@
       <c r="A47" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B47" s="23" t="s">
+      <c r="B47" s="21" t="s">
         <v>32</v>
       </c>
       <c r="C47" s="20">
@@ -2095,7 +2110,7 @@
       <c r="E47" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F47" s="22" t="s">
+      <c r="F47" s="24" t="s">
         <v>35</v>
       </c>
       <c r="G47" s="14">
@@ -2107,13 +2122,13 @@
       <c r="A48" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B48" s="24"/>
+      <c r="B48" s="22"/>
       <c r="C48" s="20">
         <v>3150</v>
       </c>
       <c r="D48" s="20"/>
       <c r="E48" s="9"/>
-      <c r="F48" s="22"/>
+      <c r="F48" s="24"/>
       <c r="G48" s="16">
         <v>3200</v>
       </c>
@@ -2123,7 +2138,7 @@
       <c r="A49" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B49" s="25"/>
+      <c r="B49" s="23"/>
       <c r="C49" s="12">
         <f>C48-C47</f>
         <v>1110</v>
@@ -2135,7 +2150,7 @@
       <c r="E49" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F49" s="22"/>
+      <c r="F49" s="24"/>
       <c r="G49" s="15">
         <f>G48-G47</f>
         <v>1100</v>
@@ -2148,7 +2163,7 @@
       <c r="A50" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B50" s="23" t="s">
+      <c r="B50" s="21" t="s">
         <v>32</v>
       </c>
       <c r="C50" s="6">
@@ -2160,7 +2175,7 @@
       <c r="E50" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F50" s="22" t="s">
+      <c r="F50" s="24" t="s">
         <v>36</v>
       </c>
       <c r="G50" s="14">
@@ -2172,13 +2187,13 @@
       <c r="A51" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B51" s="24"/>
+      <c r="B51" s="22"/>
       <c r="C51" s="3">
         <v>4500</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="9"/>
-      <c r="F51" s="22"/>
+      <c r="F51" s="24"/>
       <c r="G51" s="16">
         <v>4200</v>
       </c>
@@ -2188,7 +2203,7 @@
       <c r="A52" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B52" s="25"/>
+      <c r="B52" s="23"/>
       <c r="C52" s="12">
         <f>C51-C50</f>
         <v>1910</v>
@@ -2200,7 +2215,7 @@
       <c r="E52" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F52" s="22"/>
+      <c r="F52" s="24"/>
       <c r="G52" s="15">
         <f>G51-G50</f>
         <v>1800</v>
@@ -2227,7 +2242,7 @@
       <c r="A54" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B54" s="23" t="s">
+      <c r="B54" s="21" t="s">
         <v>37</v>
       </c>
       <c r="C54" s="6">
@@ -2239,7 +2254,7 @@
       <c r="E54" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F54" s="22" t="s">
+      <c r="F54" s="24" t="s">
         <v>38</v>
       </c>
       <c r="G54" s="14">
@@ -2253,13 +2268,13 @@
       <c r="A55" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B55" s="24"/>
+      <c r="B55" s="22"/>
       <c r="C55" s="3">
         <v>1200</v>
       </c>
       <c r="D55" s="3"/>
       <c r="E55" s="9"/>
-      <c r="F55" s="22"/>
+      <c r="F55" s="24"/>
       <c r="G55" s="16">
         <v>1200</v>
       </c>
@@ -2269,7 +2284,7 @@
       <c r="A56" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B56" s="25"/>
+      <c r="B56" s="23"/>
       <c r="C56" s="12">
         <f>C55-C54</f>
         <v>600</v>
@@ -2281,7 +2296,7 @@
       <c r="E56" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F56" s="22"/>
+      <c r="F56" s="24"/>
       <c r="G56" s="15">
         <f>G55-G54</f>
         <v>600</v>
@@ -2294,7 +2309,7 @@
       <c r="A57" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B57" s="23" t="s">
+      <c r="B57" s="21" t="s">
         <v>37</v>
       </c>
       <c r="C57" s="6">
@@ -2306,7 +2321,7 @@
       <c r="E57" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F57" s="22" t="s">
+      <c r="F57" s="24" t="s">
         <v>39</v>
       </c>
       <c r="G57" s="14">
@@ -2320,13 +2335,13 @@
       <c r="A58" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B58" s="24"/>
+      <c r="B58" s="22"/>
       <c r="C58" s="3">
         <v>2000</v>
       </c>
       <c r="D58" s="3"/>
       <c r="E58" s="9"/>
-      <c r="F58" s="22"/>
+      <c r="F58" s="24"/>
       <c r="G58" s="16">
         <v>2400</v>
       </c>
@@ -2336,7 +2351,7 @@
       <c r="A59" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B59" s="25"/>
+      <c r="B59" s="23"/>
       <c r="C59" s="12">
         <f>C58-C57</f>
         <v>1000</v>
@@ -2348,7 +2363,7 @@
       <c r="E59" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F59" s="22"/>
+      <c r="F59" s="24"/>
       <c r="G59" s="15">
         <f>G58-G57</f>
         <v>800</v>
@@ -2361,7 +2376,7 @@
       <c r="A60" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B60" s="23" t="s">
+      <c r="B60" s="21" t="s">
         <v>37</v>
       </c>
       <c r="C60" s="20">
@@ -2374,7 +2389,7 @@
       <c r="E60" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F60" s="22" t="s">
+      <c r="F60" s="24" t="s">
         <v>40</v>
       </c>
       <c r="G60" s="14">
@@ -2388,14 +2403,14 @@
       <c r="A61" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B61" s="24"/>
+      <c r="B61" s="22"/>
       <c r="C61" s="20">
         <f>2600+800</f>
         <v>3400</v>
       </c>
       <c r="D61" s="20"/>
       <c r="E61" s="9"/>
-      <c r="F61" s="22"/>
+      <c r="F61" s="24"/>
       <c r="G61" s="16">
         <v>3200</v>
       </c>
@@ -2405,7 +2420,7 @@
       <c r="A62" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B62" s="25"/>
+      <c r="B62" s="23"/>
       <c r="C62" s="12">
         <f>C61-C60</f>
         <v>1400</v>
@@ -2417,7 +2432,7 @@
       <c r="E62" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F62" s="22"/>
+      <c r="F62" s="24"/>
       <c r="G62" s="15">
         <f>G61-G60</f>
         <v>1100</v>
@@ -2430,7 +2445,7 @@
       <c r="A63" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B63" s="23" t="s">
+      <c r="B63" s="21" t="s">
         <v>37</v>
       </c>
       <c r="C63" s="6">
@@ -2443,7 +2458,7 @@
       <c r="E63" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F63" s="22" t="s">
+      <c r="F63" s="24" t="s">
         <v>41</v>
       </c>
       <c r="G63" s="14">
@@ -2457,14 +2472,14 @@
       <c r="A64" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B64" s="24"/>
+      <c r="B64" s="22"/>
       <c r="C64" s="3">
         <f>2600+1600</f>
         <v>4200</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="9"/>
-      <c r="F64" s="22"/>
+      <c r="F64" s="24"/>
       <c r="G64" s="16">
         <v>4200</v>
       </c>
@@ -2474,7 +2489,7 @@
       <c r="A65" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B65" s="25"/>
+      <c r="B65" s="23"/>
       <c r="C65" s="12">
         <f>C64-C63</f>
         <v>1740</v>
@@ -2486,7 +2501,7 @@
       <c r="E65" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F65" s="22"/>
+      <c r="F65" s="24"/>
       <c r="G65" s="15">
         <f>G64-G63</f>
         <v>1800</v>
@@ -2495,24 +2510,304 @@
         <v>23</v>
       </c>
     </row>
+    <row r="66" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G66" t="s">
+        <v>17</v>
+      </c>
+      <c r="H66" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B67" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C67" s="6">
+        <v>300</v>
+      </c>
+      <c r="D67" s="6">
+        <v>2500</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F67" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="G67" s="14">
+        <v>300</v>
+      </c>
+      <c r="H67" s="17">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B68" s="22"/>
+      <c r="C68" s="3">
+        <v>600</v>
+      </c>
+      <c r="D68" s="3"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="24"/>
+      <c r="G68" s="16">
+        <v>600</v>
+      </c>
+      <c r="H68" s="18"/>
+    </row>
+    <row r="69" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B69" s="23"/>
+      <c r="C69" s="12">
+        <f>C68-C67</f>
+        <v>300</v>
+      </c>
+      <c r="D69" s="12">
+        <f>C69/D67</f>
+        <v>0.12</v>
+      </c>
+      <c r="E69" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F69" s="24"/>
+      <c r="G69" s="15">
+        <f>G68-G67</f>
+        <v>300</v>
+      </c>
+      <c r="H69" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B70" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C70" s="6">
+        <f>480+100+100</f>
+        <v>680</v>
+      </c>
+      <c r="D70" s="6">
+        <v>2000</v>
+      </c>
+      <c r="E70" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F70" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="G70" s="14">
+        <v>600</v>
+      </c>
+      <c r="H70" s="17">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B71" s="22"/>
+      <c r="C71" s="3">
+        <f>960+150</f>
+        <v>1110</v>
+      </c>
+      <c r="D71" s="3"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="24"/>
+      <c r="G71" s="16">
+        <v>1050</v>
+      </c>
+      <c r="H71" s="18"/>
+    </row>
+    <row r="72" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B72" s="23"/>
+      <c r="C72" s="12">
+        <f>C71-C70</f>
+        <v>430</v>
+      </c>
+      <c r="D72" s="12">
+        <f>C72/D70</f>
+        <v>0.215</v>
+      </c>
+      <c r="E72" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F72" s="24"/>
+      <c r="G72" s="15">
+        <f>G71-G70</f>
+        <v>450</v>
+      </c>
+      <c r="H72" s="19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B73" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C73" s="20">
+        <f>480+200+220</f>
+        <v>900</v>
+      </c>
+      <c r="D73" s="20">
+        <v>1500</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F73" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="G73" s="14">
+        <v>900</v>
+      </c>
+      <c r="H73" s="17">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B74" s="22"/>
+      <c r="C74" s="20">
+        <f>960+450</f>
+        <v>1410</v>
+      </c>
+      <c r="D74" s="20"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="24"/>
+      <c r="G74" s="16">
+        <v>1500</v>
+      </c>
+      <c r="H74" s="18"/>
+    </row>
+    <row r="75" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B75" s="23"/>
+      <c r="C75" s="12">
+        <f>C74-C73</f>
+        <v>510</v>
+      </c>
+      <c r="D75" s="12">
+        <f>C75/D73</f>
+        <v>0.34</v>
+      </c>
+      <c r="E75" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F75" s="24"/>
+      <c r="G75" s="15">
+        <f>G74-G73</f>
+        <v>600</v>
+      </c>
+      <c r="H75" s="19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B76" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C76" s="6">
+        <f>295+220+710</f>
+        <v>1225</v>
+      </c>
+      <c r="D76" s="6">
+        <v>1000</v>
+      </c>
+      <c r="E76" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F76" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="G76" s="14">
+        <v>1200</v>
+      </c>
+      <c r="H76" s="17">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B77" s="22"/>
+      <c r="C77" s="3">
+        <f>1440+450</f>
+        <v>1890</v>
+      </c>
+      <c r="D77" s="3"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="24"/>
+      <c r="G77" s="16">
+        <v>2000</v>
+      </c>
+      <c r="H77" s="18"/>
+    </row>
+    <row r="78" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B78" s="23"/>
+      <c r="C78" s="12">
+        <f>C77-C76</f>
+        <v>665</v>
+      </c>
+      <c r="D78" s="12">
+        <f>C78/D76</f>
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="E78" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F78" s="24"/>
+      <c r="G78" s="15">
+        <f>G77-G76</f>
+        <v>800</v>
+      </c>
+      <c r="H78" s="19" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="B63:B65"/>
-    <mergeCell ref="F63:F65"/>
-    <mergeCell ref="B54:B56"/>
-    <mergeCell ref="F54:F56"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="F57:F59"/>
-    <mergeCell ref="B60:B62"/>
-    <mergeCell ref="F60:F62"/>
-    <mergeCell ref="F41:F43"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="F50:F52"/>
-    <mergeCell ref="F47:F49"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="B50:B52"/>
+  <mergeCells count="38">
+    <mergeCell ref="B76:B78"/>
+    <mergeCell ref="F76:F78"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="F67:F69"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="F70:F72"/>
+    <mergeCell ref="B73:B75"/>
+    <mergeCell ref="F73:F75"/>
     <mergeCell ref="F37:F39"/>
     <mergeCell ref="F34:F36"/>
     <mergeCell ref="N2:N4"/>
@@ -2527,6 +2822,22 @@
     <mergeCell ref="F5:F7"/>
     <mergeCell ref="F8:F10"/>
     <mergeCell ref="F11:F13"/>
+    <mergeCell ref="F41:F43"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="F50:F52"/>
+    <mergeCell ref="F47:F49"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="B63:B65"/>
+    <mergeCell ref="F63:F65"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="F54:F56"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="F57:F59"/>
+    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="F60:F62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Motor Industries Rebalance + Early PM
</commit_message>
<xml_diff>
--- a/IndustryExpanded/FACTORIES.xlsx
+++ b/IndustryExpanded/FACTORIES.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3TO_9I\Documents\Paradox Interactive\Victoria 3\mod\IndustryExpanded\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF46470F-0B1F-4183-AFFC-85767C7CA033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD6402A-5BC4-4F8E-B579-BD6663BC8926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8AEE59E-FFCD-4A72-B877-FD5D3ADEE5A1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="52">
   <si>
     <t>Building</t>
   </si>
@@ -177,6 +177,21 @@
   </si>
   <si>
     <t>Tier 3: Stranded Twisting, Rubber, Electric</t>
+  </si>
+  <si>
+    <t>Motor Industries</t>
+  </si>
+  <si>
+    <t>Tier 1: Early, No Auto</t>
+  </si>
+  <si>
+    <t>Tier 3: Hi-Psi, Electric Drive</t>
+  </si>
+  <si>
+    <t>Tier 4: Complex, Asslines</t>
+  </si>
+  <si>
+    <t>Tier 2: Steam, Pneumatic</t>
   </si>
 </sst>
 </file>
@@ -770,10 +785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{619B0D70-D2AF-46B3-9D3D-17ECB8467BBA}">
-  <dimension ref="A1:N78"/>
+  <dimension ref="A1:N93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="J82" sqref="J82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2798,16 +2813,323 @@
         <v>23</v>
       </c>
     </row>
+    <row r="79" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G79" t="s">
+        <v>17</v>
+      </c>
+      <c r="H79" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B80" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C80" s="6">
+        <v>1000</v>
+      </c>
+      <c r="D80" s="6">
+        <v>5000</v>
+      </c>
+      <c r="E80" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F80" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="G80" s="14">
+        <v>600</v>
+      </c>
+      <c r="H80" s="17">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B81" s="22"/>
+      <c r="C81" s="3">
+        <v>1620</v>
+      </c>
+      <c r="D81" s="3"/>
+      <c r="E81" s="9"/>
+      <c r="F81" s="24"/>
+      <c r="G81" s="16">
+        <v>1200</v>
+      </c>
+      <c r="H81" s="18"/>
+    </row>
+    <row r="82" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B82" s="23"/>
+      <c r="C82" s="12">
+        <f>C81-C80</f>
+        <v>620</v>
+      </c>
+      <c r="D82" s="12">
+        <f>C82/D80</f>
+        <v>0.124</v>
+      </c>
+      <c r="E82" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F82" s="24"/>
+      <c r="G82" s="15">
+        <f>G81-G80</f>
+        <v>600</v>
+      </c>
+      <c r="H82" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B83" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C83" s="6">
+        <f>1600+210</f>
+        <v>1810</v>
+      </c>
+      <c r="D83" s="6">
+        <v>4000</v>
+      </c>
+      <c r="E83" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F83" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="G83" s="14">
+        <v>1600</v>
+      </c>
+      <c r="H83" s="17">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B84" s="22"/>
+      <c r="C84" s="3">
+        <v>2700</v>
+      </c>
+      <c r="D84" s="3"/>
+      <c r="E84" s="9"/>
+      <c r="F84" s="24"/>
+      <c r="G84" s="16">
+        <v>2400</v>
+      </c>
+      <c r="H84" s="18"/>
+    </row>
+    <row r="85" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B85" s="23"/>
+      <c r="C85" s="12">
+        <f>C84-C83</f>
+        <v>890</v>
+      </c>
+      <c r="D85" s="12">
+        <f>C85/D83</f>
+        <v>0.2225</v>
+      </c>
+      <c r="E85" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F85" s="24"/>
+      <c r="G85" s="15">
+        <f>G84-G83</f>
+        <v>800</v>
+      </c>
+      <c r="H85" s="19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B86" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C86" s="20">
+        <f>1950+300</f>
+        <v>2250</v>
+      </c>
+      <c r="D86" s="20">
+        <v>3000</v>
+      </c>
+      <c r="E86" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F86" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="G86" s="14">
+        <v>2100</v>
+      </c>
+      <c r="H86" s="17">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B87" s="22"/>
+      <c r="C87" s="20">
+        <v>3300</v>
+      </c>
+      <c r="D87" s="20"/>
+      <c r="E87" s="9"/>
+      <c r="F87" s="24"/>
+      <c r="G87" s="16">
+        <v>3200</v>
+      </c>
+      <c r="H87" s="18"/>
+    </row>
+    <row r="88" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B88" s="23"/>
+      <c r="C88" s="12">
+        <f>C87-C86</f>
+        <v>1050</v>
+      </c>
+      <c r="D88" s="12">
+        <f>C88/D86</f>
+        <v>0.35</v>
+      </c>
+      <c r="E88" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F88" s="24"/>
+      <c r="G88" s="15">
+        <f>G87-G86</f>
+        <v>1100</v>
+      </c>
+      <c r="H88" s="19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B89" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C89" s="6">
+        <f>2290+495</f>
+        <v>2785</v>
+      </c>
+      <c r="D89" s="6">
+        <v>2000</v>
+      </c>
+      <c r="E89" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F89" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="G89" s="14">
+        <v>2400</v>
+      </c>
+      <c r="H89" s="17">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B90" s="22"/>
+      <c r="C90" s="3">
+        <v>4620</v>
+      </c>
+      <c r="D90" s="3"/>
+      <c r="E90" s="9"/>
+      <c r="F90" s="24"/>
+      <c r="G90" s="16">
+        <v>4200</v>
+      </c>
+      <c r="H90" s="18"/>
+    </row>
+    <row r="91" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B91" s="23"/>
+      <c r="C91" s="12">
+        <f>C90-C89</f>
+        <v>1835</v>
+      </c>
+      <c r="D91" s="12">
+        <f>C91/D89</f>
+        <v>0.91749999999999998</v>
+      </c>
+      <c r="E91" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F91" s="24"/>
+      <c r="G91" s="15">
+        <f>G90-G89</f>
+        <v>1800</v>
+      </c>
+      <c r="H91" s="19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D93">
+        <f>C90/60</f>
+        <v>77</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="B76:B78"/>
-    <mergeCell ref="F76:F78"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="F67:F69"/>
-    <mergeCell ref="B70:B72"/>
-    <mergeCell ref="F70:F72"/>
-    <mergeCell ref="B73:B75"/>
-    <mergeCell ref="F73:F75"/>
+  <mergeCells count="46">
+    <mergeCell ref="B89:B91"/>
+    <mergeCell ref="F89:F91"/>
+    <mergeCell ref="B80:B82"/>
+    <mergeCell ref="F80:F82"/>
+    <mergeCell ref="B83:B85"/>
+    <mergeCell ref="F83:F85"/>
+    <mergeCell ref="B86:B88"/>
+    <mergeCell ref="F86:F88"/>
+    <mergeCell ref="B63:B65"/>
+    <mergeCell ref="F63:F65"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="F54:F56"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="F57:F59"/>
+    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="F60:F62"/>
+    <mergeCell ref="F41:F43"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="F50:F52"/>
+    <mergeCell ref="F47:F49"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="B50:B52"/>
     <mergeCell ref="F37:F39"/>
     <mergeCell ref="F34:F36"/>
     <mergeCell ref="N2:N4"/>
@@ -2822,22 +3144,14 @@
     <mergeCell ref="F5:F7"/>
     <mergeCell ref="F8:F10"/>
     <mergeCell ref="F11:F13"/>
-    <mergeCell ref="F41:F43"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="F50:F52"/>
-    <mergeCell ref="F47:F49"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="B63:B65"/>
-    <mergeCell ref="F63:F65"/>
-    <mergeCell ref="B54:B56"/>
-    <mergeCell ref="F54:F56"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="F57:F59"/>
-    <mergeCell ref="B60:B62"/>
-    <mergeCell ref="F60:F62"/>
+    <mergeCell ref="B76:B78"/>
+    <mergeCell ref="F76:F78"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="F67:F69"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="F70:F72"/>
+    <mergeCell ref="B73:B75"/>
+    <mergeCell ref="F73:F75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Wealth 10-14 Consume Luxury Drinks, Lower Wine Weight
</commit_message>
<xml_diff>
--- a/IndustryExpanded/FACTORIES.xlsx
+++ b/IndustryExpanded/FACTORIES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3TO_9I\Documents\Paradox Interactive\Victoria 3\mod\IndustryExpanded\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD6402A-5BC4-4F8E-B579-BD6663BC8926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47749CF5-62AD-485A-99EE-A59EFDB06BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8AEE59E-FFCD-4A72-B877-FD5D3ADEE5A1}"/>
   </bookViews>
@@ -787,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{619B0D70-D2AF-46B3-9D3D-17ECB8467BBA}">
   <dimension ref="A1:N93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="J82" sqref="J82"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3106,30 +3106,14 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="B89:B91"/>
-    <mergeCell ref="F89:F91"/>
-    <mergeCell ref="B80:B82"/>
-    <mergeCell ref="F80:F82"/>
-    <mergeCell ref="B83:B85"/>
-    <mergeCell ref="F83:F85"/>
-    <mergeCell ref="B86:B88"/>
-    <mergeCell ref="F86:F88"/>
-    <mergeCell ref="B63:B65"/>
-    <mergeCell ref="F63:F65"/>
-    <mergeCell ref="B54:B56"/>
-    <mergeCell ref="F54:F56"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="F57:F59"/>
-    <mergeCell ref="B60:B62"/>
-    <mergeCell ref="F60:F62"/>
-    <mergeCell ref="F41:F43"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="F50:F52"/>
-    <mergeCell ref="F47:F49"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="B76:B78"/>
+    <mergeCell ref="F76:F78"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="F67:F69"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="F70:F72"/>
+    <mergeCell ref="B73:B75"/>
+    <mergeCell ref="F73:F75"/>
     <mergeCell ref="F37:F39"/>
     <mergeCell ref="F34:F36"/>
     <mergeCell ref="N2:N4"/>
@@ -3144,14 +3128,30 @@
     <mergeCell ref="F5:F7"/>
     <mergeCell ref="F8:F10"/>
     <mergeCell ref="F11:F13"/>
-    <mergeCell ref="B76:B78"/>
-    <mergeCell ref="F76:F78"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="F67:F69"/>
-    <mergeCell ref="B70:B72"/>
-    <mergeCell ref="F70:F72"/>
-    <mergeCell ref="B73:B75"/>
-    <mergeCell ref="F73:F75"/>
+    <mergeCell ref="F41:F43"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="F50:F52"/>
+    <mergeCell ref="F47:F49"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="B63:B65"/>
+    <mergeCell ref="F63:F65"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="F54:F56"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="F57:F59"/>
+    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="F60:F62"/>
+    <mergeCell ref="B89:B91"/>
+    <mergeCell ref="F89:F91"/>
+    <mergeCell ref="B80:B82"/>
+    <mergeCell ref="F80:F82"/>
+    <mergeCell ref="B83:B85"/>
+    <mergeCell ref="F83:F85"/>
+    <mergeCell ref="B86:B88"/>
+    <mergeCell ref="F86:F88"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rebalance Wiremill, Furniture, Tools, Chemical, Glass
</commit_message>
<xml_diff>
--- a/IndustryExpanded/FACTORIES.xlsx
+++ b/IndustryExpanded/FACTORIES.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3TO_9I\Documents\Paradox Interactive\Victoria 3\mod\IndustryExpanded\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47749CF5-62AD-485A-99EE-A59EFDB06BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BCDF74-D9D6-4F0C-98AF-8797488C4AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8AEE59E-FFCD-4A72-B877-FD5D3ADEE5A1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="64">
   <si>
     <t>Building</t>
   </si>
@@ -140,15 +140,6 @@
     <t>Tier 1: Handcrafting</t>
   </si>
   <si>
-    <t>Tier 2: Lathe, watertube</t>
-  </si>
-  <si>
-    <t>Tier 3:Mechanized, Electric Drive</t>
-  </si>
-  <si>
-    <t>Tier 4: Plastic, Asslines</t>
-  </si>
-  <si>
     <t>Glassworks</t>
   </si>
   <si>
@@ -158,40 +149,85 @@
     <t>Tier 2: Leaded, Wooden Utens</t>
   </si>
   <si>
-    <t>Tier 3: Crystal, Metallic, Rollers</t>
-  </si>
-  <si>
-    <t>Tier 4: Crystal, Plastic, Blowers</t>
-  </si>
-  <si>
     <t>Wiremill</t>
   </si>
   <si>
-    <t>Tier 4: Electroplated, Rubber, Asslines</t>
-  </si>
-  <si>
-    <t>Tier 1: Solid Wire, Copper Cable, Manual</t>
-  </si>
-  <si>
-    <t>Tier 2: Stranded Twisting, Insulated, Pneumatic</t>
-  </si>
-  <si>
-    <t>Tier 3: Stranded Twisting, Rubber, Electric</t>
-  </si>
-  <si>
     <t>Motor Industries</t>
   </si>
   <si>
-    <t>Tier 1: Early, No Auto</t>
-  </si>
-  <si>
-    <t>Tier 3: Hi-Psi, Electric Drive</t>
-  </si>
-  <si>
-    <t>Tier 4: Complex, Asslines</t>
-  </si>
-  <si>
-    <t>Tier 2: Steam, Pneumatic</t>
+    <t>Tier 4: Plastic</t>
+  </si>
+  <si>
+    <t>Tier 3:Mechanized</t>
+  </si>
+  <si>
+    <t>Tier 2: Lathe</t>
+  </si>
+  <si>
+    <t>0,1-0,12</t>
+  </si>
+  <si>
+    <t>0,16-0,18</t>
+  </si>
+  <si>
+    <t>0,21-0,24</t>
+  </si>
+  <si>
+    <t>0,34-0,38</t>
+  </si>
+  <si>
+    <t>Tier 4: Crystal, Plastic</t>
+  </si>
+  <si>
+    <t>Tier 3: Crystal, Metallic</t>
+  </si>
+  <si>
+    <t>Chemical Plants</t>
+  </si>
+  <si>
+    <t>Tier 1: Artificial</t>
+  </si>
+  <si>
+    <t>Tier 2: Improved</t>
+  </si>
+  <si>
+    <t>Tier 3:Nitrogen</t>
+  </si>
+  <si>
+    <t>MIN EMPL:</t>
+  </si>
+  <si>
+    <t>MAX AUTO COST</t>
+  </si>
+  <si>
+    <t>THR BONUS</t>
+  </si>
+  <si>
+    <t>MAX PROD P/E</t>
+  </si>
+  <si>
+    <t>Tier 4: Complex</t>
+  </si>
+  <si>
+    <t>Tier 3: Hi-Psi</t>
+  </si>
+  <si>
+    <t>Tier 2: Steam</t>
+  </si>
+  <si>
+    <t>Tier 1: Early</t>
+  </si>
+  <si>
+    <t>Tier 1: Solid Wire, Copper Cable</t>
+  </si>
+  <si>
+    <t>Tier 2: Stranded Twisting, Insulated</t>
+  </si>
+  <si>
+    <t>Tier 3: Stranded Twisting, Rubber</t>
+  </si>
+  <si>
+    <t>Tier 4: Electroplated, Rubber</t>
   </si>
 </sst>
 </file>
@@ -208,7 +244,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -293,8 +329,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -382,11 +442,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
@@ -431,6 +506,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -442,6 +526,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -785,10 +882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{619B0D70-D2AF-46B3-9D3D-17ECB8467BBA}">
-  <dimension ref="A1:N93"/>
+  <dimension ref="A1:N133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,6 +900,7 @@
     <col min="9" max="9" width="15" customWidth="1"/>
     <col min="10" max="10" width="18.42578125" customWidth="1"/>
     <col min="11" max="11" width="10.42578125" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" customWidth="1"/>
     <col min="14" max="14" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -842,7 +940,7 @@
       <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="27" t="s">
         <v>8</v>
       </c>
       <c r="G2" s="14">
@@ -864,7 +962,7 @@
       <c r="M2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="24" t="s">
+      <c r="N2" s="27" t="s">
         <v>13</v>
       </c>
     </row>
@@ -880,7 +978,7 @@
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="24"/>
+      <c r="F3" s="27"/>
       <c r="G3" s="16">
         <v>1200</v>
       </c>
@@ -897,7 +995,7 @@
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="9"/>
-      <c r="N3" s="24"/>
+      <c r="N3" s="27"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
@@ -917,7 +1015,7 @@
       <c r="E4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="24"/>
+      <c r="F4" s="27"/>
       <c r="G4" s="15">
         <f>G3-G2</f>
         <v>600</v>
@@ -942,7 +1040,7 @@
       <c r="M4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="24"/>
+      <c r="N4" s="27"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -961,7 +1059,7 @@
       <c r="E5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="27" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="14">
@@ -984,7 +1082,7 @@
       <c r="M5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="N5" s="24" t="s">
+      <c r="N5" s="27" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1001,7 +1099,7 @@
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="24"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="16">
         <v>2400</v>
       </c>
@@ -1017,7 +1115,7 @@
       </c>
       <c r="L6" s="3"/>
       <c r="M6" s="9"/>
-      <c r="N6" s="24"/>
+      <c r="N6" s="27"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -1037,7 +1135,7 @@
       <c r="E7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="24"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="15">
         <f>G6-G5</f>
         <v>800</v>
@@ -1062,7 +1160,7 @@
       <c r="M7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="N7" s="24"/>
+      <c r="N7" s="27"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -1081,7 +1179,7 @@
       <c r="E8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="27" t="s">
         <v>10</v>
       </c>
       <c r="G8" s="14">
@@ -1104,7 +1202,7 @@
       <c r="M8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="N8" s="24" t="s">
+      <c r="N8" s="27" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1121,7 +1219,7 @@
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="9"/>
-      <c r="F9" s="24"/>
+      <c r="F9" s="27"/>
       <c r="G9" s="16">
         <v>3200</v>
       </c>
@@ -1138,7 +1236,7 @@
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="9"/>
-      <c r="N9" s="24"/>
+      <c r="N9" s="27"/>
     </row>
     <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
@@ -1158,7 +1256,7 @@
       <c r="E10" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="24"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="15">
         <f>G9-G8</f>
         <v>1100</v>
@@ -1183,7 +1281,7 @@
       <c r="M10" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="N10" s="24"/>
+      <c r="N10" s="27"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
@@ -1202,7 +1300,7 @@
       <c r="E11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="24" t="s">
+      <c r="F11" s="27" t="s">
         <v>11</v>
       </c>
       <c r="G11" s="14">
@@ -1225,7 +1323,7 @@
       <c r="M11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="N11" s="24" t="s">
+      <c r="N11" s="27" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1242,7 +1340,7 @@
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="9"/>
-      <c r="F12" s="24"/>
+      <c r="F12" s="27"/>
       <c r="G12" s="16">
         <v>4200</v>
       </c>
@@ -1259,7 +1357,7 @@
       </c>
       <c r="L12" s="3"/>
       <c r="M12" s="9"/>
-      <c r="N12" s="24"/>
+      <c r="N12" s="27"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
@@ -1279,7 +1377,7 @@
       <c r="E13" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="24"/>
+      <c r="F13" s="27"/>
       <c r="G13" s="15">
         <f>G12-G11</f>
         <v>1800</v>
@@ -1304,7 +1402,7 @@
       <c r="M13" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="N13" s="24"/>
+      <c r="N13" s="27"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
@@ -1340,7 +1438,7 @@
       <c r="E15" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="24" t="s">
+      <c r="F15" s="27" t="s">
         <v>26</v>
       </c>
       <c r="G15" s="14">
@@ -1376,7 +1474,7 @@
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="9"/>
-      <c r="F16" s="24"/>
+      <c r="F16" s="27"/>
       <c r="G16" s="16">
         <v>1200</v>
       </c>
@@ -1411,7 +1509,7 @@
       <c r="E17" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="24"/>
+      <c r="F17" s="27"/>
       <c r="G17" s="15">
         <f>G16-G15</f>
         <v>600</v>
@@ -1453,7 +1551,7 @@
       <c r="E18" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="24" t="s">
+      <c r="F18" s="27" t="s">
         <v>25</v>
       </c>
       <c r="G18" s="14">
@@ -1490,7 +1588,7 @@
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="9"/>
-      <c r="F19" s="24"/>
+      <c r="F19" s="27"/>
       <c r="G19" s="16">
         <v>2400</v>
       </c>
@@ -1526,7 +1624,7 @@
       <c r="E20" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F20" s="24"/>
+      <c r="F20" s="27"/>
       <c r="G20" s="15">
         <f>G19-G18</f>
         <v>800</v>
@@ -1660,7 +1758,7 @@
       <c r="E24" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="24" t="s">
+      <c r="F24" s="27" t="s">
         <v>27</v>
       </c>
       <c r="G24" s="14">
@@ -1689,7 +1787,7 @@
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="9"/>
-      <c r="F25" s="24"/>
+      <c r="F25" s="27"/>
       <c r="G25" s="16">
         <v>4200</v>
       </c>
@@ -1719,7 +1817,7 @@
       <c r="E26" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="24"/>
+      <c r="F26" s="27"/>
       <c r="G26" s="15">
         <f>G25-G24</f>
         <v>1800</v>
@@ -1788,7 +1886,7 @@
       <c r="E31" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="24" t="s">
+      <c r="F31" s="27" t="s">
         <v>29</v>
       </c>
       <c r="G31" s="14">
@@ -1805,7 +1903,7 @@
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="9"/>
-      <c r="F32" s="24"/>
+      <c r="F32" s="27"/>
       <c r="G32" s="16">
         <v>2400</v>
       </c>
@@ -1827,7 +1925,7 @@
       <c r="E33" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F33" s="24"/>
+      <c r="F33" s="27"/>
       <c r="G33" s="15">
         <f>G32-G31</f>
         <v>800</v>
@@ -1851,7 +1949,7 @@
       <c r="E34" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F34" s="25" t="s">
+      <c r="F34" s="28" t="s">
         <v>31</v>
       </c>
       <c r="G34" s="14">
@@ -1869,7 +1967,7 @@
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="9"/>
-      <c r="F35" s="25"/>
+      <c r="F35" s="28"/>
       <c r="G35" s="16">
         <v>3200</v>
       </c>
@@ -1891,7 +1989,7 @@
       <c r="E36" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F36" s="25"/>
+      <c r="F36" s="28"/>
       <c r="G36" s="15">
         <f>G35-G34</f>
         <v>1100</v>
@@ -1915,7 +2013,7 @@
       <c r="E37" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F37" s="25" t="s">
+      <c r="F37" s="28" t="s">
         <v>30</v>
       </c>
       <c r="G37" s="14">
@@ -1932,7 +2030,7 @@
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="9"/>
-      <c r="F38" s="25"/>
+      <c r="F38" s="28"/>
       <c r="G38" s="16">
         <v>4200</v>
       </c>
@@ -1954,7 +2052,7 @@
       <c r="E39" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F39" s="25"/>
+      <c r="F39" s="28"/>
       <c r="G39" s="15">
         <f>G38-G37</f>
         <v>1800</v>
@@ -1981,11 +2079,11 @@
       <c r="A41" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C41" s="6">
-        <v>800</v>
+        <v>660</v>
       </c>
       <c r="D41" s="6">
         <v>5000</v>
@@ -1993,7 +2091,7 @@
       <c r="E41" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F41" s="24" t="s">
+      <c r="F41" s="27" t="s">
         <v>33</v>
       </c>
       <c r="G41" s="14">
@@ -2005,13 +2103,13 @@
       <c r="A42" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B42" s="22"/>
+      <c r="B42" s="25"/>
       <c r="C42" s="3">
-        <v>1350</v>
+        <v>1200</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="9"/>
-      <c r="F42" s="24"/>
+      <c r="F42" s="27"/>
       <c r="G42" s="16">
         <v>1200</v>
       </c>
@@ -2021,49 +2119,48 @@
       <c r="A43" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="23"/>
+      <c r="B43" s="26"/>
       <c r="C43" s="12">
         <f>C42-C41</f>
-        <v>550</v>
+        <v>540</v>
       </c>
       <c r="D43" s="12">
         <f>C43/D41</f>
-        <v>0.11</v>
+        <v>0.108</v>
       </c>
       <c r="E43" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F43" s="24"/>
+      <c r="F43" s="27"/>
       <c r="G43" s="15">
         <f>G42-G41</f>
         <v>600</v>
       </c>
       <c r="H43" s="19" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B44" s="21" t="s">
+      <c r="B44" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C44" s="6">
-        <f>1000+280</f>
-        <v>1280</v>
+        <v>1200</v>
       </c>
       <c r="D44" s="6">
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F44" s="24" t="s">
-        <v>34</v>
+      <c r="F44" s="27" t="s">
+        <v>41</v>
       </c>
       <c r="G44" s="14">
-        <v>1600</v>
+        <v>1200</v>
       </c>
       <c r="H44" s="17"/>
     </row>
@@ -2071,15 +2168,15 @@
       <c r="A45" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B45" s="22"/>
+      <c r="B45" s="25"/>
       <c r="C45" s="3">
-        <v>2100</v>
+        <v>2010</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="9"/>
-      <c r="F45" s="24"/>
+      <c r="F45" s="27"/>
       <c r="G45" s="16">
-        <v>2400</v>
+        <v>2000</v>
       </c>
       <c r="H45" s="18"/>
     </row>
@@ -2087,49 +2184,48 @@
       <c r="A46" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="23"/>
+      <c r="B46" s="26"/>
       <c r="C46" s="12">
         <f>C45-C44</f>
-        <v>820</v>
+        <v>810</v>
       </c>
       <c r="D46" s="12">
         <f>C46/D44</f>
-        <v>0.20499999999999999</v>
+        <v>0.16200000000000001</v>
       </c>
       <c r="E46" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F46" s="24"/>
+      <c r="F46" s="27"/>
       <c r="G46" s="15">
         <f>G45-G44</f>
         <v>800</v>
       </c>
       <c r="H46" s="19" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B47" s="21" t="s">
+      <c r="B47" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C47" s="20">
-        <f>1620+420</f>
-        <v>2040</v>
-      </c>
-      <c r="D47" s="20">
-        <v>3000</v>
+        <v>1800</v>
+      </c>
+      <c r="D47" s="6">
+        <v>5000</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F47" s="24" t="s">
-        <v>35</v>
+      <c r="F47" s="27" t="s">
+        <v>40</v>
       </c>
       <c r="G47" s="14">
-        <v>2100</v>
+        <v>1800</v>
       </c>
       <c r="H47" s="17"/>
     </row>
@@ -2137,15 +2233,15 @@
       <c r="A48" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B48" s="22"/>
+      <c r="B48" s="25"/>
       <c r="C48" s="20">
-        <v>3150</v>
+        <v>2880</v>
       </c>
       <c r="D48" s="20"/>
       <c r="E48" s="9"/>
-      <c r="F48" s="24"/>
+      <c r="F48" s="27"/>
       <c r="G48" s="16">
-        <v>3200</v>
+        <v>2900</v>
       </c>
       <c r="H48" s="18"/>
     </row>
@@ -2153,45 +2249,45 @@
       <c r="A49" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B49" s="23"/>
+      <c r="B49" s="26"/>
       <c r="C49" s="12">
         <f>C48-C47</f>
-        <v>1110</v>
+        <v>1080</v>
       </c>
       <c r="D49" s="12">
         <f>C49/D47</f>
-        <v>0.37</v>
+        <v>0.216</v>
       </c>
       <c r="E49" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F49" s="24"/>
+      <c r="F49" s="27"/>
       <c r="G49" s="15">
         <f>G48-G47</f>
         <v>1100</v>
       </c>
       <c r="H49" s="19" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B50" s="21" t="s">
+      <c r="B50" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C50" s="6">
-        <v>2590</v>
+        <v>2400</v>
       </c>
       <c r="D50" s="6">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="E50" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F50" s="24" t="s">
-        <v>36</v>
+      <c r="F50" s="27" t="s">
+        <v>39</v>
       </c>
       <c r="G50" s="14">
         <v>2400</v>
@@ -2202,13 +2298,13 @@
       <c r="A51" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B51" s="22"/>
+      <c r="B51" s="25"/>
       <c r="C51" s="3">
-        <v>4500</v>
+        <v>4200</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="9"/>
-      <c r="F51" s="24"/>
+      <c r="F51" s="27"/>
       <c r="G51" s="16">
         <v>4200</v>
       </c>
@@ -2218,25 +2314,25 @@
       <c r="A52" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B52" s="23"/>
+      <c r="B52" s="26"/>
       <c r="C52" s="12">
         <f>C51-C50</f>
-        <v>1910</v>
+        <v>1800</v>
       </c>
       <c r="D52" s="12">
         <f>C52/D50</f>
-        <v>0.95499999999999996</v>
+        <v>0.36</v>
       </c>
       <c r="E52" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F52" s="24"/>
+      <c r="F52" s="27"/>
       <c r="G52" s="15">
         <f>G51-G50</f>
         <v>1800</v>
       </c>
       <c r="H52" s="19" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2257,39 +2353,37 @@
       <c r="A54" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B54" s="21" t="s">
-        <v>37</v>
+      <c r="B54" s="24" t="s">
+        <v>34</v>
       </c>
       <c r="C54" s="6">
         <v>600</v>
       </c>
       <c r="D54" s="6">
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="E54" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F54" s="24" t="s">
-        <v>38</v>
+      <c r="F54" s="27" t="s">
+        <v>35</v>
       </c>
       <c r="G54" s="14">
         <v>600</v>
       </c>
-      <c r="H54" s="17">
-        <v>5000</v>
-      </c>
+      <c r="H54" s="17"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B55" s="22"/>
+      <c r="B55" s="25"/>
       <c r="C55" s="3">
         <v>1200</v>
       </c>
       <c r="D55" s="3"/>
       <c r="E55" s="9"/>
-      <c r="F55" s="24"/>
+      <c r="F55" s="27"/>
       <c r="G55" s="16">
         <v>1200</v>
       </c>
@@ -2299,36 +2393,37 @@
       <c r="A56" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B56" s="23"/>
+      <c r="B56" s="26"/>
       <c r="C56" s="12">
         <f>C55-C54</f>
         <v>600</v>
       </c>
       <c r="D56" s="12">
         <f>C56/D54</f>
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
       <c r="E56" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F56" s="24"/>
+      <c r="F56" s="27"/>
       <c r="G56" s="15">
         <f>G55-G54</f>
         <v>600</v>
       </c>
       <c r="H56" s="19" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B57" s="21" t="s">
-        <v>37</v>
+      <c r="B57" s="24" t="s">
+        <v>34</v>
       </c>
       <c r="C57" s="6">
-        <v>1000</v>
+        <f>800+400</f>
+        <v>1200</v>
       </c>
       <c r="D57" s="6">
         <v>5000</v>
@@ -2336,29 +2431,28 @@
       <c r="E57" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F57" s="24" t="s">
-        <v>39</v>
+      <c r="F57" s="27" t="s">
+        <v>36</v>
       </c>
       <c r="G57" s="14">
-        <v>1600</v>
-      </c>
-      <c r="H57" s="17">
-        <v>4000</v>
-      </c>
+        <v>1200</v>
+      </c>
+      <c r="H57" s="17"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B58" s="22"/>
+      <c r="B58" s="25"/>
       <c r="C58" s="3">
+        <f>1440+560</f>
         <v>2000</v>
       </c>
       <c r="D58" s="3"/>
       <c r="E58" s="9"/>
-      <c r="F58" s="24"/>
+      <c r="F58" s="27"/>
       <c r="G58" s="16">
-        <v>2400</v>
+        <v>2000</v>
       </c>
       <c r="H58" s="18"/>
     </row>
@@ -2366,68 +2460,66 @@
       <c r="A59" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B59" s="23"/>
+      <c r="B59" s="26"/>
       <c r="C59" s="12">
         <f>C58-C57</f>
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="D59" s="12">
         <f>C59/D57</f>
-        <v>0.2</v>
+        <v>0.16</v>
       </c>
       <c r="E59" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F59" s="24"/>
+      <c r="F59" s="27"/>
       <c r="G59" s="15">
         <f>G58-G57</f>
         <v>800</v>
       </c>
       <c r="H59" s="19" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B60" s="21" t="s">
-        <v>37</v>
+      <c r="B60" s="24" t="s">
+        <v>34</v>
       </c>
       <c r="C60" s="20">
-        <f>1400+400+200</f>
-        <v>2000</v>
-      </c>
-      <c r="D60" s="20">
-        <v>3500</v>
+        <f>1200+500</f>
+        <v>1700</v>
+      </c>
+      <c r="D60" s="6">
+        <v>5000</v>
       </c>
       <c r="E60" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F60" s="24" t="s">
-        <v>40</v>
+      <c r="F60" s="27" t="s">
+        <v>47</v>
       </c>
       <c r="G60" s="14">
-        <v>2100</v>
-      </c>
-      <c r="H60" s="17">
-        <v>3000</v>
-      </c>
+        <v>1800</v>
+      </c>
+      <c r="H60" s="17"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B61" s="22"/>
+      <c r="B61" s="25"/>
       <c r="C61" s="20">
-        <f>2600+800</f>
-        <v>3400</v>
+        <f>2000+900</f>
+        <v>2900</v>
       </c>
       <c r="D61" s="20"/>
       <c r="E61" s="9"/>
-      <c r="F61" s="24"/>
+      <c r="F61" s="27"/>
       <c r="G61" s="16">
-        <v>3200</v>
+        <v>2900</v>
       </c>
       <c r="H61" s="18"/>
     </row>
@@ -2435,66 +2527,64 @@
       <c r="A62" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B62" s="23"/>
+      <c r="B62" s="26"/>
       <c r="C62" s="12">
         <f>C61-C60</f>
-        <v>1400</v>
+        <v>1200</v>
       </c>
       <c r="D62" s="12">
         <f>C62/D60</f>
-        <v>0.4</v>
+        <v>0.24</v>
       </c>
       <c r="E62" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F62" s="24"/>
+      <c r="F62" s="27"/>
       <c r="G62" s="15">
         <f>G61-G60</f>
         <v>1100</v>
       </c>
       <c r="H62" s="19" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B63" s="21" t="s">
-        <v>37</v>
+      <c r="B63" s="24" t="s">
+        <v>34</v>
       </c>
       <c r="C63" s="6">
-        <f>1400+700+360</f>
-        <v>2460</v>
+        <f>1200+800</f>
+        <v>2000</v>
       </c>
       <c r="D63" s="6">
-        <v>2000</v>
+        <v>4500</v>
       </c>
       <c r="E63" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F63" s="24" t="s">
-        <v>41</v>
+      <c r="F63" s="27" t="s">
+        <v>46</v>
       </c>
       <c r="G63" s="14">
         <v>2400</v>
       </c>
-      <c r="H63" s="17">
-        <v>2000</v>
-      </c>
+      <c r="H63" s="17"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B64" s="22"/>
+      <c r="B64" s="25"/>
       <c r="C64" s="3">
-        <f>2600+1600</f>
-        <v>4200</v>
+        <f>2000+1600</f>
+        <v>3600</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="9"/>
-      <c r="F64" s="24"/>
+      <c r="F64" s="27"/>
       <c r="G64" s="16">
         <v>4200</v>
       </c>
@@ -2504,25 +2594,25 @@
       <c r="A65" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B65" s="23"/>
+      <c r="B65" s="26"/>
       <c r="C65" s="12">
         <f>C64-C63</f>
-        <v>1740</v>
+        <v>1600</v>
       </c>
       <c r="D65" s="12">
         <f>C65/D63</f>
-        <v>0.87</v>
+        <v>0.35555555555555557</v>
       </c>
       <c r="E65" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F65" s="24"/>
+      <c r="F65" s="27"/>
       <c r="G65" s="15">
         <f>G64-G63</f>
         <v>1800</v>
       </c>
       <c r="H65" s="19" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2543,41 +2633,39 @@
       <c r="A67" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B67" s="21" t="s">
-        <v>42</v>
+      <c r="B67" s="24" t="s">
+        <v>37</v>
       </c>
       <c r="C67" s="6">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="D67" s="6">
-        <v>2500</v>
+        <v>5000</v>
       </c>
       <c r="E67" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F67" s="24" t="s">
-        <v>44</v>
+      <c r="F67" s="27" t="s">
+        <v>60</v>
       </c>
       <c r="G67" s="14">
-        <v>300</v>
-      </c>
-      <c r="H67" s="17">
-        <v>2500</v>
-      </c>
+        <v>600</v>
+      </c>
+      <c r="H67" s="17"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B68" s="22"/>
+      <c r="B68" s="25"/>
       <c r="C68" s="3">
-        <v>600</v>
+        <v>1200</v>
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="9"/>
-      <c r="F68" s="24"/>
+      <c r="F68" s="27"/>
       <c r="G68" s="16">
-        <v>600</v>
+        <v>1200</v>
       </c>
       <c r="H68" s="18"/>
     </row>
@@ -2585,10 +2673,10 @@
       <c r="A69" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B69" s="23"/>
+      <c r="B69" s="26"/>
       <c r="C69" s="12">
         <f>C68-C67</f>
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="D69" s="12">
         <f>C69/D67</f>
@@ -2597,56 +2685,54 @@
       <c r="E69" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F69" s="24"/>
+      <c r="F69" s="27"/>
       <c r="G69" s="15">
         <f>G68-G67</f>
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="H69" s="19" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B70" s="21" t="s">
-        <v>42</v>
+      <c r="B70" s="24" t="s">
+        <v>37</v>
       </c>
       <c r="C70" s="6">
-        <f>480+100+100</f>
-        <v>680</v>
+        <f>900+300</f>
+        <v>1200</v>
       </c>
       <c r="D70" s="6">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="E70" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F70" s="24" t="s">
-        <v>45</v>
+      <c r="F70" s="27" t="s">
+        <v>61</v>
       </c>
       <c r="G70" s="14">
-        <v>600</v>
-      </c>
-      <c r="H70" s="17">
-        <v>2000</v>
-      </c>
+        <v>1200</v>
+      </c>
+      <c r="H70" s="17"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B71" s="22"/>
+      <c r="B71" s="25"/>
       <c r="C71" s="3">
-        <f>960+150</f>
-        <v>1110</v>
+        <f>1605+405</f>
+        <v>2010</v>
       </c>
       <c r="D71" s="3"/>
       <c r="E71" s="9"/>
-      <c r="F71" s="24"/>
+      <c r="F71" s="27"/>
       <c r="G71" s="16">
-        <v>1050</v>
+        <v>2000</v>
       </c>
       <c r="H71" s="18"/>
     </row>
@@ -2654,68 +2740,66 @@
       <c r="A72" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B72" s="23"/>
+      <c r="B72" s="26"/>
       <c r="C72" s="12">
         <f>C71-C70</f>
-        <v>430</v>
+        <v>810</v>
       </c>
       <c r="D72" s="12">
         <f>C72/D70</f>
-        <v>0.215</v>
+        <v>0.16200000000000001</v>
       </c>
       <c r="E72" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F72" s="24"/>
+      <c r="F72" s="27"/>
       <c r="G72" s="15">
         <f>G71-G70</f>
-        <v>450</v>
+        <v>800</v>
       </c>
       <c r="H72" s="19" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B73" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C73" s="20">
-        <f>480+200+220</f>
-        <v>900</v>
-      </c>
-      <c r="D73" s="20">
+      <c r="B73" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C73" s="6">
+        <f>900+600</f>
         <v>1500</v>
       </c>
+      <c r="D73" s="6">
+        <v>5000</v>
+      </c>
       <c r="E73" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F73" s="24" t="s">
-        <v>46</v>
+      <c r="F73" s="27" t="s">
+        <v>62</v>
       </c>
       <c r="G73" s="14">
-        <v>900</v>
-      </c>
-      <c r="H73" s="17">
-        <v>1500</v>
-      </c>
+        <v>1800</v>
+      </c>
+      <c r="H73" s="17"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B74" s="22"/>
+      <c r="B74" s="25"/>
       <c r="C74" s="20">
-        <f>960+450</f>
-        <v>1410</v>
+        <f>1605+900</f>
+        <v>2505</v>
       </c>
       <c r="D74" s="20"/>
       <c r="E74" s="9"/>
-      <c r="F74" s="24"/>
+      <c r="F74" s="27"/>
       <c r="G74" s="16">
-        <v>1500</v>
+        <v>2900</v>
       </c>
       <c r="H74" s="18"/>
     </row>
@@ -2723,68 +2807,66 @@
       <c r="A75" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B75" s="23"/>
+      <c r="B75" s="26"/>
       <c r="C75" s="12">
         <f>C74-C73</f>
-        <v>510</v>
+        <v>1005</v>
       </c>
       <c r="D75" s="12">
         <f>C75/D73</f>
-        <v>0.34</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="E75" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F75" s="24"/>
+      <c r="F75" s="27"/>
       <c r="G75" s="15">
         <f>G74-G73</f>
-        <v>600</v>
+        <v>1100</v>
       </c>
       <c r="H75" s="19" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B76" s="21" t="s">
-        <v>42</v>
+      <c r="B76" s="24" t="s">
+        <v>37</v>
       </c>
       <c r="C76" s="6">
-        <f>295+220+710</f>
-        <v>1225</v>
+        <f>1710+600</f>
+        <v>2310</v>
       </c>
       <c r="D76" s="6">
-        <v>1000</v>
+        <v>5000</v>
       </c>
       <c r="E76" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F76" s="24" t="s">
-        <v>43</v>
+      <c r="F76" s="27" t="s">
+        <v>63</v>
       </c>
       <c r="G76" s="14">
-        <v>1200</v>
-      </c>
-      <c r="H76" s="17">
-        <v>1000</v>
-      </c>
+        <v>2400</v>
+      </c>
+      <c r="H76" s="17"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B77" s="22"/>
-      <c r="C77" s="3">
-        <f>1440+450</f>
-        <v>1890</v>
+      <c r="B77" s="25"/>
+      <c r="C77" s="20">
+        <f>3300+900</f>
+        <v>4200</v>
       </c>
       <c r="D77" s="3"/>
       <c r="E77" s="9"/>
-      <c r="F77" s="24"/>
+      <c r="F77" s="27"/>
       <c r="G77" s="16">
-        <v>2000</v>
+        <v>4200</v>
       </c>
       <c r="H77" s="18"/>
     </row>
@@ -2792,328 +2874,636 @@
       <c r="A78" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B78" s="23"/>
+      <c r="B78" s="26"/>
       <c r="C78" s="12">
         <f>C77-C76</f>
-        <v>665</v>
+        <v>1890</v>
       </c>
       <c r="D78" s="12">
         <f>C78/D76</f>
-        <v>0.66500000000000004</v>
+        <v>0.378</v>
       </c>
       <c r="E78" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F78" s="24"/>
+      <c r="F78" s="27"/>
       <c r="G78" s="15">
         <f>G77-G76</f>
+        <v>1800</v>
+      </c>
+      <c r="H78" s="19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B79" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C79" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="D79" s="34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="33">
+        <v>2500</v>
+      </c>
+      <c r="B80" s="33">
+        <v>495</v>
+      </c>
+      <c r="C80" s="33">
+        <v>0.2</v>
+      </c>
+      <c r="D80" s="35">
+        <f>((C77*(1+C80))-(C76*(1+C80)+B80))/A80</f>
+        <v>0.70920000000000005</v>
+      </c>
+    </row>
+    <row r="93" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I93" s="31"/>
+      <c r="J93" s="31"/>
+      <c r="K93" s="31"/>
+      <c r="L93" s="31"/>
+    </row>
+    <row r="94" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I94" s="30"/>
+      <c r="J94" s="30"/>
+      <c r="K94" s="30"/>
+      <c r="L94" s="30"/>
+    </row>
+    <row r="107" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B107" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G107" t="s">
+        <v>17</v>
+      </c>
+      <c r="H107" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B108" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C108" s="6"/>
+      <c r="D108" s="6">
+        <v>5000</v>
+      </c>
+      <c r="E108" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F108" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="G108" s="14">
+        <v>600</v>
+      </c>
+      <c r="H108" s="17">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B109" s="25"/>
+      <c r="C109" s="3"/>
+      <c r="D109" s="3"/>
+      <c r="E109" s="9"/>
+      <c r="F109" s="27"/>
+      <c r="G109" s="16">
+        <v>1200</v>
+      </c>
+      <c r="H109" s="18"/>
+    </row>
+    <row r="110" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B110" s="26"/>
+      <c r="C110" s="12">
+        <f>C109-C108</f>
+        <v>0</v>
+      </c>
+      <c r="D110" s="12">
+        <f>C110/D108</f>
+        <v>0</v>
+      </c>
+      <c r="E110" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F110" s="27"/>
+      <c r="G110" s="15">
+        <f>G109-G108</f>
+        <v>600</v>
+      </c>
+      <c r="H110" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B111" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C111" s="6"/>
+      <c r="D111" s="6">
+        <v>5000</v>
+      </c>
+      <c r="E111" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F111" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="G111" s="14">
+        <v>1600</v>
+      </c>
+      <c r="H111" s="17">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B112" s="25"/>
+      <c r="C112" s="3"/>
+      <c r="D112" s="3"/>
+      <c r="E112" s="9"/>
+      <c r="F112" s="27"/>
+      <c r="G112" s="16">
+        <v>2400</v>
+      </c>
+      <c r="H112" s="18"/>
+    </row>
+    <row r="113" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B113" s="26"/>
+      <c r="C113" s="12">
+        <f>C112-C111</f>
+        <v>0</v>
+      </c>
+      <c r="D113" s="12">
+        <f>C113/D111</f>
+        <v>0</v>
+      </c>
+      <c r="E113" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F113" s="27"/>
+      <c r="G113" s="15">
+        <f>G112-G111</f>
         <v>800</v>
       </c>
-      <c r="H78" s="19" t="s">
+      <c r="H113" s="19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A114" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B114" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C114" s="20"/>
+      <c r="D114" s="6">
+        <v>5000</v>
+      </c>
+      <c r="E114" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F114" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="G114" s="14">
+        <v>2100</v>
+      </c>
+      <c r="H114" s="17">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B115" s="25"/>
+      <c r="C115" s="20"/>
+      <c r="D115" s="20"/>
+      <c r="E115" s="9"/>
+      <c r="F115" s="27"/>
+      <c r="G115" s="16">
+        <v>3200</v>
+      </c>
+      <c r="H115" s="18"/>
+    </row>
+    <row r="116" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B116" s="26"/>
+      <c r="C116" s="12">
+        <f>C115-C114</f>
+        <v>0</v>
+      </c>
+      <c r="D116" s="12">
+        <f>C116/D114</f>
+        <v>0</v>
+      </c>
+      <c r="E116" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F116" s="27"/>
+      <c r="G116" s="15">
+        <f>G115-G114</f>
+        <v>1100</v>
+      </c>
+      <c r="H116" s="19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A117" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B117" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C117" s="6"/>
+      <c r="D117" s="6">
+        <v>5000</v>
+      </c>
+      <c r="E117" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F117" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="G117" s="14">
+        <v>2400</v>
+      </c>
+      <c r="H117" s="17">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A118" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B118" s="25"/>
+      <c r="C118" s="3"/>
+      <c r="D118" s="3"/>
+      <c r="E118" s="9"/>
+      <c r="F118" s="27"/>
+      <c r="G118" s="16">
+        <v>4200</v>
+      </c>
+      <c r="H118" s="18"/>
+    </row>
+    <row r="119" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B119" s="26"/>
+      <c r="C119" s="12">
+        <f>C118-C117</f>
+        <v>0</v>
+      </c>
+      <c r="D119" s="12">
+        <f>C119/D117</f>
+        <v>0</v>
+      </c>
+      <c r="E119" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F119" s="27"/>
+      <c r="G119" s="15">
+        <f>G118-G117</f>
+        <v>1800</v>
+      </c>
+      <c r="H119" s="19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="1" t="s">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A120" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B120" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C120" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="D120" s="34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A121" s="33">
+        <v>3000</v>
+      </c>
+      <c r="B121" s="33">
+        <v>420</v>
+      </c>
+      <c r="C121" s="33">
+        <v>0.15</v>
+      </c>
+      <c r="D121" s="35">
+        <f>((C118*(1+C121))-(C117*(1+C121)+B121))/A121</f>
+        <v>-0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B122" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F79" s="2" t="s">
+      <c r="F122" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G79" t="s">
+      <c r="G122" t="s">
         <v>17</v>
       </c>
-      <c r="H79" t="s">
+      <c r="H122" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B80" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C80" s="6">
-        <v>1000</v>
-      </c>
-      <c r="D80" s="6">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A123" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B123" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C123" s="6">
+        <v>1300</v>
+      </c>
+      <c r="D123" s="6">
         <v>5000</v>
       </c>
-      <c r="E80" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F80" s="24" t="s">
+      <c r="E123" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F123" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="G123" s="14">
+        <v>1200</v>
+      </c>
+      <c r="H123" s="17">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A124" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B124" s="20"/>
+      <c r="C124" s="3">
+        <v>2100</v>
+      </c>
+      <c r="D124" s="3"/>
+      <c r="E124" s="9"/>
+      <c r="F124" s="23"/>
+      <c r="G124" s="16">
+        <v>2000</v>
+      </c>
+      <c r="H124" s="18"/>
+    </row>
+    <row r="125" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B125" s="22"/>
+      <c r="C125" s="12">
+        <f>C124-C123</f>
+        <v>800</v>
+      </c>
+      <c r="D125" s="12">
+        <f>C125/D123</f>
+        <v>0.16</v>
+      </c>
+      <c r="E125" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F125" s="23"/>
+      <c r="G125" s="15">
+        <f>G124-G123</f>
+        <v>800</v>
+      </c>
+      <c r="H125" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A126" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B126" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="G80" s="14">
-        <v>600</v>
-      </c>
-      <c r="H80" s="17">
+      <c r="C126" s="6">
+        <v>1900</v>
+      </c>
+      <c r="D126" s="6">
         <v>5000</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B81" s="22"/>
-      <c r="C81" s="3">
-        <v>1620</v>
-      </c>
-      <c r="D81" s="3"/>
-      <c r="E81" s="9"/>
-      <c r="F81" s="24"/>
-      <c r="G81" s="16">
-        <v>1200</v>
-      </c>
-      <c r="H81" s="18"/>
-    </row>
-    <row r="82" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B82" s="23"/>
-      <c r="C82" s="12">
-        <f>C81-C80</f>
-        <v>620</v>
-      </c>
-      <c r="D82" s="12">
-        <f>C82/D80</f>
-        <v>0.124</v>
-      </c>
-      <c r="E82" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F82" s="24"/>
-      <c r="G82" s="15">
-        <f>G81-G80</f>
-        <v>600</v>
-      </c>
-      <c r="H82" s="19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B83" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C83" s="6">
-        <f>1600+210</f>
-        <v>1810</v>
-      </c>
-      <c r="D83" s="6">
-        <v>4000</v>
-      </c>
-      <c r="E83" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F83" s="24" t="s">
+      <c r="E126" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F126" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="G126" s="14">
+        <v>1800</v>
+      </c>
+      <c r="H126" s="17">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A127" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B127" s="25"/>
+      <c r="C127" s="3">
+        <v>3000</v>
+      </c>
+      <c r="D127" s="3"/>
+      <c r="E127" s="9"/>
+      <c r="F127" s="27"/>
+      <c r="G127" s="16">
+        <v>2900</v>
+      </c>
+      <c r="H127" s="18"/>
+    </row>
+    <row r="128" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B128" s="26"/>
+      <c r="C128" s="12">
+        <f>C127-C126</f>
+        <v>1100</v>
+      </c>
+      <c r="D128" s="12">
+        <f>C128/D126</f>
+        <v>0.22</v>
+      </c>
+      <c r="E128" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F128" s="27"/>
+      <c r="G128" s="15">
+        <f>G127-G126</f>
+        <v>1100</v>
+      </c>
+      <c r="H128" s="19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A129" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B129" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C129" s="20">
+        <v>2500</v>
+      </c>
+      <c r="D129" s="6">
+        <v>5000</v>
+      </c>
+      <c r="E129" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F129" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="G83" s="14">
-        <v>1600</v>
-      </c>
-      <c r="H83" s="17">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B84" s="22"/>
-      <c r="C84" s="3">
-        <v>2700</v>
-      </c>
-      <c r="D84" s="3"/>
-      <c r="E84" s="9"/>
-      <c r="F84" s="24"/>
-      <c r="G84" s="16">
-        <v>2400</v>
-      </c>
-      <c r="H84" s="18"/>
-    </row>
-    <row r="85" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B85" s="23"/>
-      <c r="C85" s="12">
-        <f>C84-C83</f>
-        <v>890</v>
-      </c>
-      <c r="D85" s="12">
-        <f>C85/D83</f>
-        <v>0.2225</v>
-      </c>
-      <c r="E85" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F85" s="24"/>
-      <c r="G85" s="15">
-        <f>G84-G83</f>
-        <v>800</v>
-      </c>
-      <c r="H85" s="19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B86" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C86" s="20">
-        <f>1950+300</f>
-        <v>2250</v>
-      </c>
-      <c r="D86" s="20">
+      <c r="G129" s="14">
+        <v>2500</v>
+      </c>
+      <c r="H129" s="17">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A130" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B130" s="25"/>
+      <c r="C130" s="20">
+        <v>4500</v>
+      </c>
+      <c r="D130" s="20"/>
+      <c r="E130" s="9"/>
+      <c r="F130" s="27"/>
+      <c r="G130" s="16">
+        <v>4500</v>
+      </c>
+      <c r="H130" s="18"/>
+    </row>
+    <row r="131" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B131" s="26"/>
+      <c r="C131" s="12">
+        <v>1900</v>
+      </c>
+      <c r="D131" s="12">
+        <f>C131/D129</f>
+        <v>0.38</v>
+      </c>
+      <c r="E131" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F131" s="27"/>
+      <c r="G131" s="15">
+        <f>G130-G129</f>
+        <v>2000</v>
+      </c>
+      <c r="H131" s="19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A132" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B132" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C132" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="D132" s="34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A133" s="33">
         <v>3000</v>
       </c>
-      <c r="E86" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F86" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="G86" s="14">
-        <v>2100</v>
-      </c>
-      <c r="H86" s="17">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B87" s="22"/>
-      <c r="C87" s="20">
-        <v>3300</v>
-      </c>
-      <c r="D87" s="20"/>
-      <c r="E87" s="9"/>
-      <c r="F87" s="24"/>
-      <c r="G87" s="16">
-        <v>3200</v>
-      </c>
-      <c r="H87" s="18"/>
-    </row>
-    <row r="88" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B88" s="23"/>
-      <c r="C88" s="12">
-        <f>C87-C86</f>
-        <v>1050</v>
-      </c>
-      <c r="D88" s="12">
-        <f>C88/D86</f>
-        <v>0.35</v>
-      </c>
-      <c r="E88" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F88" s="24"/>
-      <c r="G88" s="15">
-        <f>G87-G86</f>
-        <v>1100</v>
-      </c>
-      <c r="H88" s="19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B89" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C89" s="6">
-        <f>2290+495</f>
-        <v>2785</v>
-      </c>
-      <c r="D89" s="6">
-        <v>2000</v>
-      </c>
-      <c r="E89" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F89" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="G89" s="14">
-        <v>2400</v>
-      </c>
-      <c r="H89" s="17">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B90" s="22"/>
-      <c r="C90" s="3">
-        <v>4620</v>
-      </c>
-      <c r="D90" s="3"/>
-      <c r="E90" s="9"/>
-      <c r="F90" s="24"/>
-      <c r="G90" s="16">
-        <v>4200</v>
-      </c>
-      <c r="H90" s="18"/>
-    </row>
-    <row r="91" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B91" s="23"/>
-      <c r="C91" s="12">
-        <f>C90-C89</f>
-        <v>1835</v>
-      </c>
-      <c r="D91" s="12">
-        <f>C91/D89</f>
-        <v>0.91749999999999998</v>
-      </c>
-      <c r="E91" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F91" s="24"/>
-      <c r="G91" s="15">
-        <f>G90-G89</f>
-        <v>1800</v>
-      </c>
-      <c r="H91" s="19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D93">
-        <f>C90/60</f>
-        <v>77</v>
+      <c r="B133" s="33">
+        <v>420</v>
+      </c>
+      <c r="C133" s="33">
+        <v>0.15</v>
+      </c>
+      <c r="D133" s="35">
+        <f>((C130*(1+C133))-(C129*(1+C133)+B133))/A133</f>
+        <v>0.62666666666666671</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="46">
-    <mergeCell ref="B76:B78"/>
-    <mergeCell ref="F76:F78"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="F67:F69"/>
-    <mergeCell ref="B70:B72"/>
-    <mergeCell ref="F70:F72"/>
-    <mergeCell ref="B73:B75"/>
-    <mergeCell ref="F73:F75"/>
+  <mergeCells count="50">
+    <mergeCell ref="B126:B128"/>
+    <mergeCell ref="F126:F128"/>
+    <mergeCell ref="B129:B131"/>
+    <mergeCell ref="F129:F131"/>
+    <mergeCell ref="B117:B119"/>
+    <mergeCell ref="F117:F119"/>
+    <mergeCell ref="B108:B110"/>
+    <mergeCell ref="F108:F110"/>
+    <mergeCell ref="B111:B113"/>
+    <mergeCell ref="F111:F113"/>
+    <mergeCell ref="B114:B116"/>
+    <mergeCell ref="F114:F116"/>
+    <mergeCell ref="B63:B65"/>
+    <mergeCell ref="F63:F65"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="F54:F56"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="F57:F59"/>
+    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="F60:F62"/>
+    <mergeCell ref="F41:F43"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="F50:F52"/>
+    <mergeCell ref="F47:F49"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="B50:B52"/>
     <mergeCell ref="F37:F39"/>
     <mergeCell ref="F34:F36"/>
     <mergeCell ref="N2:N4"/>
@@ -3128,30 +3518,14 @@
     <mergeCell ref="F5:F7"/>
     <mergeCell ref="F8:F10"/>
     <mergeCell ref="F11:F13"/>
-    <mergeCell ref="F41:F43"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="F50:F52"/>
-    <mergeCell ref="F47:F49"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="B63:B65"/>
-    <mergeCell ref="F63:F65"/>
-    <mergeCell ref="B54:B56"/>
-    <mergeCell ref="F54:F56"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="F57:F59"/>
-    <mergeCell ref="B60:B62"/>
-    <mergeCell ref="F60:F62"/>
-    <mergeCell ref="B89:B91"/>
-    <mergeCell ref="F89:F91"/>
-    <mergeCell ref="B80:B82"/>
-    <mergeCell ref="F80:F82"/>
-    <mergeCell ref="B83:B85"/>
-    <mergeCell ref="F83:F85"/>
-    <mergeCell ref="B86:B88"/>
-    <mergeCell ref="F86:F88"/>
+    <mergeCell ref="B76:B78"/>
+    <mergeCell ref="F76:F78"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="F67:F69"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="F70:F72"/>
+    <mergeCell ref="B73:B75"/>
+    <mergeCell ref="F73:F75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>